<commit_message>
fonte, about e foto
</commit_message>
<xml_diff>
--- a/frontend/src/data/products.xlsx
+++ b/frontend/src/data/products.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3cc8a21b1ba9f6fb/Desktop/Drop da Mari/Drop da Mari - Emergent React/Drop da Mari/frontend/src/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Conta Teste\OneDrive\Desktop\Projetos Dev\Drop da Mari\Drop da Mari\frontend\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="434" documentId="11_B08ABFDBB4B9E9D8F7F21EF40234A1444B4E3C9E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{34745EFF-1DBE-46D0-B536-02425C0078F1}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67884F10-DBAF-4BB3-9D75-762B8521F0BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="198">
   <si>
     <t>id</t>
   </si>
@@ -58,12 +58,6 @@
     <t>Pré-treino True Energyzer</t>
   </si>
   <si>
-    <t>Boné Esportivo 5 Panel</t>
-  </si>
-  <si>
-    <t>Cinta Porta Numeral e Gel</t>
-  </si>
-  <si>
     <t>Leve, limpo, natural e delicioso!</t>
   </si>
   <si>
@@ -605,6 +599,21 @@
   </si>
   <si>
     <t>Sofisticação com conforto ao seu treino.</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/dupz0ffvs/image/upload/v1759169761/Gel_de_Limpeza_Facial_All_Clean_pw2t0l.webp</t>
+  </si>
+  <si>
+    <t>https://kesserstore.com.br/products/gel-de-limpeza-facial-all-clean</t>
+  </si>
+  <si>
+    <t>Gel de limpeza facial Kesser All Clean</t>
+  </si>
+  <si>
+    <t>Boné Esportivo Yopp 5 Panel</t>
+  </si>
+  <si>
+    <t>Cinta Porta Numeral e Gel Yopp</t>
   </si>
 </sst>
 </file>
@@ -694,16 +703,16 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <top style="thin">
+        <bottom style="thin">
           <color auto="1"/>
-        </top>
+        </bottom>
       </border>
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
+        <top style="thin">
           <color auto="1"/>
-        </bottom>
+        </top>
       </border>
     </dxf>
     <dxf>
@@ -748,13 +757,9 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9423426A-FF74-4080-A8AC-F983F8483237}" name="Tabela1" displayName="Tabela1" ref="A1:H47" totalsRowShown="0" headerRowDxfId="4" headerRowBorderDxfId="3" tableBorderDxfId="2">
-  <autoFilter ref="A1:H47" xr:uid="{9423426A-FF74-4080-A8AC-F983F8483237}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9423426A-FF74-4080-A8AC-F983F8483237}" name="Tabela1" displayName="Tabela1" ref="A1:H48" totalsRowShown="0" headerRowDxfId="4" headerRowBorderDxfId="2" tableBorderDxfId="3">
+  <autoFilter ref="A1:H48" xr:uid="{9423426A-FF74-4080-A8AC-F983F8483237}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A22:H38">
     <sortCondition ref="H1:H38"/>
   </sortState>
@@ -1059,10 +1064,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H47"/>
+  <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1105,278 +1110,278 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>12</v>
+        <v>196</v>
       </c>
       <c r="C6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C9" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C10" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>13</v>
+        <v>197</v>
       </c>
       <c r="C11" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H11" t="s">
         <v>32</v>
-      </c>
-      <c r="H11" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C12" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C13" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1384,160 +1389,160 @@
         <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E14" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F14" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" t="s">
         <v>36</v>
       </c>
-      <c r="C15" t="s">
-        <v>37</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E15" t="s">
-        <v>23</v>
-      </c>
-      <c r="F15" t="s">
-        <v>38</v>
-      </c>
       <c r="G15" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H15" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C16" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E16" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F16" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H16" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C17" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E17" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F17" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H17" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" t="s">
+        <v>126</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E18" t="s">
+        <v>21</v>
+      </c>
+      <c r="F18" t="s">
+        <v>23</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H18" t="s">
         <v>41</v>
-      </c>
-      <c r="C18" t="s">
-        <v>128</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E18" t="s">
-        <v>23</v>
-      </c>
-      <c r="F18" t="s">
-        <v>25</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="H18" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C19" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E19" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F19" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H19" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
+        <v>127</v>
+      </c>
+      <c r="C20" t="s">
         <v>129</v>
       </c>
-      <c r="C20" t="s">
-        <v>131</v>
-      </c>
       <c r="D20" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E20" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F20" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H20" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
@@ -1545,22 +1550,22 @@
         <v>10</v>
       </c>
       <c r="C21" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E21" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F21" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H21" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
@@ -1568,22 +1573,22 @@
         <v>8</v>
       </c>
       <c r="C22" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E22" t="s">
+        <v>20</v>
+      </c>
+      <c r="F22" t="s">
         <v>22</v>
       </c>
-      <c r="F22" t="s">
-        <v>24</v>
-      </c>
       <c r="G22" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H22" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
@@ -1591,574 +1596,591 @@
         <v>11</v>
       </c>
       <c r="C23" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E23" t="s">
+        <v>20</v>
+      </c>
+      <c r="F23" t="s">
         <v>22</v>
       </c>
-      <c r="F23" t="s">
-        <v>24</v>
-      </c>
       <c r="G23" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="H23" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C24" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E24" t="s">
+        <v>20</v>
+      </c>
+      <c r="F24" t="s">
         <v>22</v>
       </c>
-      <c r="F24" t="s">
-        <v>24</v>
-      </c>
       <c r="G24" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H24" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C25" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E25" t="s">
+        <v>20</v>
+      </c>
+      <c r="F25" t="s">
         <v>22</v>
       </c>
-      <c r="F25" t="s">
-        <v>24</v>
-      </c>
       <c r="G25" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H25" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C26" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E26" t="s">
+        <v>20</v>
+      </c>
+      <c r="F26" t="s">
         <v>22</v>
       </c>
-      <c r="F26" t="s">
-        <v>24</v>
-      </c>
       <c r="G26" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H26" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C27" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E27" t="s">
+        <v>20</v>
+      </c>
+      <c r="F27" t="s">
         <v>22</v>
       </c>
-      <c r="F27" t="s">
-        <v>24</v>
-      </c>
       <c r="G27" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H27" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C28" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E28" t="s">
+        <v>20</v>
+      </c>
+      <c r="F28" t="s">
         <v>22</v>
       </c>
-      <c r="F28" t="s">
-        <v>24</v>
-      </c>
       <c r="G28" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H28" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C29" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E29" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F29" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H29" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C30" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E30" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F30" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H30" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C31" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E31" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F31" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H31" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C32" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E32" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F32" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="H32" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C33" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E33" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F33" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="H33" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C34" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E34" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F34" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H34" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C35" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E35" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F35" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H35" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C36" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E36" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F36" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="H36" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C37" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E37" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F37" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="H37" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C38" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E38" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F38" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="H38" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C39" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E39" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F39" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="H39" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C40" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E40" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F40" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="H40" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C41" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E41" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F41" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="H41" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C42" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E42" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F42" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="H42" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C43" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E43" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F43" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="H43" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C44" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E44" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F44" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="H44" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C45" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E45" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F45" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="H45" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C46" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E46" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F46" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G46" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="H46" t="s">
         <v>148</v>
-      </c>
-      <c r="H46" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C47" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E47" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F47" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="H47" t="s">
-        <v>150</v>
+        <v>148</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>195</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="F48" t="s">
+        <v>36</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="H48" t="s">
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -2239,10 +2261,11 @@
     <hyperlink ref="G44" r:id="rId74" xr:uid="{ED0A3F82-A547-4243-B8DD-33BCB25FE521}"/>
     <hyperlink ref="G45" r:id="rId75" xr:uid="{10B6A68A-2347-4926-B04F-8A82D4563FEF}"/>
     <hyperlink ref="G46" r:id="rId76" xr:uid="{38F23661-6621-461A-8FBC-3B0D8B1EC316}"/>
+    <hyperlink ref="D48" r:id="rId77" xr:uid="{243D949C-60EE-4D16-B3A0-D0934B7A271D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId77"/>
+    <tablePart r:id="rId78"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>